<commit_message>
UNAGI Japanese Assortment - 3297676809 업데이트
</commit_message>
<xml_diff>
--- a/Data/UNA/UNAGI Japanese Assortment - 3297676809/3297676809.xlsx
+++ b/Data/UNA/UNAGI Japanese Assortment - 3297676809/3297676809.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Pull Request Here\UNAGI Japanese Assortment 鰻の和風箱 - 3297676809\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\UNAGI Japanese Assortment - 3297676809\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466647DF-0820-41DD-9B16-69F615BDCF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50198B4-83BB-46DB-8E06-302579C96B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240925" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-29에 새로 추가된 노드들 (4개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="134">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -53,42 +76,42 @@
     <t>和風の髪</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본식 머리</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HairDef+UNAGIwahuukami2.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>일본식 머리</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>UNAGIwahuukami2.label</t>
   </si>
   <si>
     <t>和風ロング</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본식 긴머리</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAGIkamikazari.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>일본식 긴머리</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>ThingDef</t>
   </si>
   <si>
@@ -98,90 +121,102 @@
     <t>UNA 和風髪飾り</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>카미카자리</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAGIkamikazari.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>카미카자리</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>UNAGIkamikazari.description</t>
   </si>
   <si>
     <t>和風の髪飾りです。少しだけ頭を保護します。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본식 머리장식입니다. 머리를 아주 약간 보호해줍니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_UNAjingasa.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>일본식 머리장식입니다. 머리를 아주 약간 보호해줍니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_UNAjingasa.label</t>
   </si>
   <si>
     <t>UNA 陣笠</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>진가사</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_UNAjingasa.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>진가사</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_UNAjingasa.description</t>
   </si>
   <si>
     <t>ヘルメットと同じように使える陣笠です。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헬멧처럼 사용할 수 있는 일본식 머리 방어구입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAwasitagi.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>헬멧처럼 사용할 수 있는 일본식 머리 방어구입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>UNAwasitagi.description</t>
   </si>
   <si>
     <t>バニラの襟付きシャツと同じように扱える着物です。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>티셔츠와 동일한 성능의 의복입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAwasitagi.label</t>
   </si>
   <si>
@@ -192,7 +227,7 @@
         <rFont val="맑은 고딕"/>
         <family val="2"/>
       </rPr>
-      <t>티셔츠와 동일한 성능의 의복입니다.</t>
+      <t>UNAwasitagi.label</t>
     </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -207,7 +242,7 @@
         <rFont val="맑은 고딕"/>
         <family val="2"/>
       </rPr>
-      <t>UNAwasitagi.label</t>
+      <t>유카타</t>
     </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -215,24 +250,24 @@
     <t>ThingDef+Apparel_UNAwahaori.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>유카타</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_UNAwahaori.description</t>
   </si>
   <si>
     <t>シンプルな羽織です。バニラのダスターコートと同じ性能です。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>바람막이와 동일한 성능의 겉옷입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_UNAwahaori.label</t>
   </si>
   <si>
@@ -243,7 +278,7 @@
         <rFont val="맑은 고딕"/>
         <family val="2"/>
       </rPr>
-      <t>바람막이와 동일한 성능의 겉옷입니다.</t>
+      <t>Apparel_UNAwahaori.label</t>
     </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -258,7 +293,7 @@
         <rFont val="맑은 고딕"/>
         <family val="2"/>
       </rPr>
-      <t>Apparel_UNAwahaori.label</t>
+      <t>바람막이 하오리</t>
     </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -266,442 +301,482 @@
     <t>ThingDef+Apparel_UNAwaboudan.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>바람막이 하오리</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_UNAwaboudan.label</t>
   </si>
   <si>
     <t>UNA 防弾軽甲冑</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방탄 갑주</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_UNAwaboudan.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>방탄 갑주</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_UNAwaboudan.description</t>
   </si>
   <si>
     <t>バニラの防弾チョッキと同じ性能の、軽めの甲冑です。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방탄조끼와 동일한 성능의 가벼운 갑옷입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAkariginu.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>방탄조끼와 동일한 성능의 가벼운 갑옷입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>UNAkariginu.label</t>
   </si>
   <si>
     <t>UNA 狩衣</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>카리기누</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAkariginu.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>카리기누</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>UNAkariginu.description</t>
   </si>
   <si>
     <t>歴史的に高位の方が身に着けていた装束です。もちろん、この星でも貴族の人に満足して貰えます。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+      </rPr>
+      <t>주로 고위 계급에서 사용하던 복장입니다. 물론 변방계의 귀족들에게도 만족스러운 옷입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+UNAGItyazukin.label</t>
   </si>
   <si>
+    <t>UNAGItyazukin.label</t>
+  </si>
+  <si>
+    <t>UNA 涼しい利休帽</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>기치즈킨</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNAGItyazukin.description</t>
+  </si>
+  <si>
+    <t>UNAGItyazukin.description</t>
+  </si>
+  <si>
+    <t>利休帽と呼ばれる帽子。性能はカウボーイハットと同じです。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이휴모라고도 불리는 모자입니다. 성능은 카우보이 모자와 동일합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNAhokkamuri.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>UNAhokkamuri.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA あったかほっかむり</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>호카무리</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNAhokkamuri.description</t>
+  </si>
+  <si>
+    <t>UNAhokkamuri.description</t>
+  </si>
+  <si>
+    <t>農家の人がよく使うほっかむり。ニット帽とおなじように暖かいです。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>농부들이 주로 사용하는 털모자입니다. 생긴 모양에 걸맞게 따뜻합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNAtatiebosi.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>UNAtatiebosi.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA 烏帽子</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>에보시</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNAtatiebosi.description</t>
+  </si>
+  <si>
+    <t>UNAtatiebosi.description</t>
+  </si>
+  <si>
+    <t>貴族の方が被れる帽子です。寒さと暑さを少し防ぎます。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>귀족들이 쓰는 모자입니다. 추위와 더위를 약간 막아줍니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Inuhariko.label</t>
+  </si>
+  <si>
+    <t>UNA 犬張り子置物</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>UNA_Inuhariko.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Inuhariko.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>강아지 인형</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA_Inuhariko.description</t>
+  </si>
+  <si>
+    <t>日本の伝統的な犬の置物です。</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_okimonomini.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본의 전통적인 개 인형입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA 置物（小）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>UNA_okimonomini.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+UNA_okimonomini.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>소형 일본 장식품</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA_okimonomini.description</t>
+  </si>
+  <si>
+    <t>日本の伝統的な置物のセットです。4種類の絵柄があります。回転させることで好きな絵柄に変えられます。</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_watyokoku.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본 전통 인형으로, 4종류의 형상을 지니고 있습니다. 회전을 통해 다양한 모습으로 표시할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA_watyokoku.label</t>
+  </si>
+  <si>
+    <t>UNA Japanese sculpture</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_watyokoku.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본풍 조각상</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA_watyokoku.description</t>
+  </si>
+  <si>
+    <t>Sculptures in the form of figurines familiar to Japanese people. It can be rotated to display any picture you like.</t>
+  </si>
+  <si>
+    <t>ThingDef+UNAdotera.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>일본인에게 친숙한 피규어 형태의 조형물입니다. 회전을 통해 다양한 모습으로 표시할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNAdotera.label</t>
+  </si>
+  <si>
+    <t>UNA どてら</t>
+  </si>
+  <si>
+    <t>ThingDef+UNAdotera.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>도테라</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNAdotera.description</t>
+  </si>
+  <si>
+    <t>日本の伝統的な上着で、寒い日に羽織ります。綿でふわふわ暖かいです。</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Genkankazari.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>추운 날에 입는 일본 전통 겉옷으로, 면으로 만들어져 보송보송하고 따뜻합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNA_Genkankazari.label</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Genkankazari.description</t>
+  </si>
+  <si>
+    <t>UNA_Genkankazari.description</t>
+  </si>
+  <si>
+    <t>日本の伝統的な正月飾りです。</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Kadomatu.label</t>
+  </si>
+  <si>
+    <t>UNA_Kadomatu.label</t>
+  </si>
+  <si>
+    <t>UNA 門松</t>
+  </si>
+  <si>
+    <t>ThingDef+UNA_Kadomatu.description</t>
+  </si>
+  <si>
+    <t>UNA_Kadomatu.description</t>
+  </si>
+  <si>
+    <r>
+      <t>UNA 玄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>関</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
-      </rPr>
-      <t>주로 고위 계급에서 사용하던 복장입니다. 물론 변방계의 귀족들에게도 만족스러운 옷입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAGItyazukin.label</t>
-  </si>
-  <si>
-    <t>UNA 涼しい利休帽</t>
-  </si>
-  <si>
-    <t>ThingDef+UNAGItyazukin.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>기치즈킨</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAGItyazukin.description</t>
-  </si>
-  <si>
-    <t>利休帽と呼ばれる帽子。性能はカウボーイハットと同じです。</t>
-  </si>
-  <si>
-    <t>ThingDef+UNAhokkamuri.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>이휴모라고도 불리는 모자입니다. 성능은 카우보이 모자와 동일합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNA あったかほっかむり</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>UNAhokkamuri.label</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+UNAhokkamuri.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>호카무리</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAhokkamuri.description</t>
-  </si>
-  <si>
-    <t>農家の人がよく使うほっかむり。ニット帽とおなじように暖かいです。</t>
-  </si>
-  <si>
-    <t>ThingDef+UNAtatiebosi.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>농부들이 주로 사용하는 털모자입니다. 생긴 모양에 걸맞게 따뜻합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNA 烏帽子</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>UNAtatiebosi.label</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+UNAtatiebosi.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>에보시</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAtatiebosi.description</t>
-  </si>
-  <si>
-    <t>貴族の方が被れる帽子です。寒さと暑さを少し防ぎます。</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_Inuhariko.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>귀족들이 쓰는 모자입니다. 추위와 더위를 약간 막아줍니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNA 犬張り子置物</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_Inuhariko.description</t>
-  </si>
-  <si>
-    <t>UNA_Inuhariko.description</t>
-  </si>
-  <si>
-    <t>日本の伝統的な犬の置物です。</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_okimonomini.label</t>
-  </si>
-  <si>
-    <t>UNA 置物（小）</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_okimonomini.description</t>
-  </si>
-  <si>
-    <t>UNA_okimonomini.description</t>
-  </si>
-  <si>
-    <t>日本の伝統的な置物のセットです。4種類の絵柄があります。回転させることで好きな絵柄に変えられます。</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_watyokoku.label</t>
-  </si>
-  <si>
-    <t>UNA_watyokoku.label</t>
-  </si>
-  <si>
-    <t>UNA Japanese sculpture</t>
-  </si>
-  <si>
-    <t>ThingDef+UNA_watyokoku.description</t>
-  </si>
-  <si>
-    <t>UNA_watyokoku.description</t>
-  </si>
-  <si>
-    <t>Sculptures in the form of figurines familiar to Japanese people. It can be rotated to display any picture you like.</t>
-  </si>
-  <si>
-    <t>ThingDef+UNAdotera.label</t>
-  </si>
-  <si>
-    <t>UNAdotera.label</t>
-  </si>
-  <si>
-    <t>UNA どてら</t>
-  </si>
-  <si>
-    <t>ThingDef+UNAdotera.description</t>
-  </si>
-  <si>
-    <t>UNAdotera.description</t>
-  </si>
-  <si>
-    <t>日本の伝統的な上着で、寒い日に羽織ります。綿でふわふわ暖かいです。</t>
-  </si>
-  <si>
-    <t>UNA_Inuhariko.label</t>
+        <charset val="129"/>
+      </rPr>
+      <t>飾り</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>강아지 인형</t>
+    <t>일본식 현관 장식</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>일본의 전통적인 개 인형입니다.</t>
+    <t>일본의 전통적인 새해 장식입니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>UNA_okimonomini.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>소형 일본 장식품</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본풍 조각상</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본인에게 친숙한 피규어 형태의 조형물입니다. 회전을 통해 다양한 모습으로 표시할 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본 전통 인형으로, 4종류의 형상을 지니고 있습니다. 회전을 통해 다양한 모습으로 표시할 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>도테라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추운 날에 입는 일본 전통 겉옷으로, 면으로 만들어져 보송보송하고 따뜻합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>귀족들이 쓰는 모자입니다. 추위와 더위를 약간 막아줍니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>에보시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAtatiebosi.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>농부들이 주로 사용하는 털모자입니다. 생긴 모양에 걸맞게 따뜻합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>호카무리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAhokkamuri.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이휴모라고도 불리는 모자입니다. 성능은 카우보이 모자와 동일합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>기치즈킨</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주로 고위 계급에서 사용하던 복장입니다. 물론 변방계의 귀족들에게도 만족스러운 옷입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>카리기누</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>방탄조끼와 동일한 성능의 가벼운 갑옷입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>방탄 갑주</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>바람막이 하오리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_UNAwahaori.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>바람막이와 동일한 성능의 겉옷입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>유카타</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNAwasitagi.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>티셔츠와 동일한 성능의 의복입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>헬멧처럼 사용할 수 있는 일본식 머리 방어구입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>진가사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본식 머리장식입니다. 머리를 아주 약간 보호해줍니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>카미카자리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본식 긴머리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일본식 머리</t>
+    <t>카도마츠</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -709,7 +784,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,6 +820,19 @@
       <sz val="8"/>
       <name val="돋움"/>
       <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="새굴림"/>
+      <family val="1"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -1079,11 +1167,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1094,7 +1182,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="69.08984375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1131,12 +1220,12 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1148,12 +1237,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1165,12 +1254,12 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -1182,12 +1271,12 @@
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -1199,12 +1288,12 @@
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -1216,12 +1305,12 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -1233,29 +1322,29 @@
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1267,29 +1356,29 @@
         <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1301,12 +1390,12 @@
         <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1318,12 +1407,12 @@
         <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -1335,12 +1424,12 @@
         <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1352,12 +1441,12 @@
         <v>62</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -1369,12 +1458,12 @@
         <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -1386,29 +1475,29 @@
         <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
@@ -1420,29 +1509,29 @@
         <v>78</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
@@ -1454,148 +1543,217 @@
         <v>86</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>119</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1653,12 +1811,12 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1670,12 +1828,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1687,12 +1845,12 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -1704,12 +1862,12 @@
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -1721,12 +1879,12 @@
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -1738,12 +1896,12 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -1755,29 +1913,29 @@
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>137</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1789,29 +1947,29 @@
         <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1823,12 +1981,12 @@
         <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1840,12 +1998,12 @@
         <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -1857,12 +2015,12 @@
         <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1874,12 +2032,12 @@
         <v>62</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>128</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -1891,12 +2049,12 @@
         <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -1908,29 +2066,29 @@
         <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
@@ -1942,29 +2100,29 @@
         <v>78</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
@@ -1976,7 +2134,7 @@
         <v>86</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>